<commit_message>
Updated Good Description, Correct values
</commit_message>
<xml_diff>
--- a/TANI 595_details.xlsx
+++ b/TANI 595_details.xlsx
@@ -461,32 +461,32 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>HSN/SAC</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Company Name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Invoice No</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Date of Invoice</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>GSTIN NO</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>GSTIN</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>HSN/SAC</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RICE</t>
+          <t>RICE</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -533,77 +533,50 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>30.00</t>
+          <t>30</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,200</t>
+          <t>441</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>TANISHQ AGRO INDUSTRIES</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>595</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>01-08-2023</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>27AAKPW5971G1Z1</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>23AACCA8432H1ZY</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>10063090</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
-LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
-EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
-VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>SINGH TRANSPORT</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NL01AB4849</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>9380MP41</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>7772825143</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> RICE</t>
+          <t>RICE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -618,72 +591,45 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5,700</t>
+          <t>441</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>TANISHQ AGRO INDUSTRIES</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>595</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>01-08-2023</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>27AAKPW5971G1Z1</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>23AACCA8432H1ZY</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>10063090</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
-LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
-EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
-VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>SINGH TRANSPORT</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>NL01AB4849</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>9380MP41</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>7772825143</t>
-        </is>
-      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>